<commit_message>
DA Jenkins Build readiness - Master
</commit_message>
<xml_diff>
--- a/src/test/java/Database/Reference Documents/DA_GIT.xlsx
+++ b/src/test/java/Database/Reference Documents/DA_GIT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syadav12\Automation_WorkSpace\src\test\java\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syadav12\Automation_WorkSpace\src\test\java\Database\Reference Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A39B43-82C3-492E-B6B3-CEA7E8EEF3EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D246FBF-2D67-408F-B660-0F5D657A06DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11775" windowHeight="7830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1368,12 +1368,6 @@
     <t>crmrec2</t>
   </si>
   <si>
-    <t xml:space="preserve">Armando	</t>
-  </si>
-  <si>
-    <t>Bowers</t>
-  </si>
-  <si>
     <t>Sara</t>
   </si>
   <si>
@@ -1414,6 +1408,12 @@
   </si>
   <si>
     <t>Fox</t>
+  </si>
+  <si>
+    <t>spijgsdj</t>
+  </si>
+  <si>
+    <t>skdjfspdjf</t>
   </si>
 </sst>
 </file>
@@ -2334,7 +2334,7 @@
                   <a14:compatExt spid="_x0000_s41985"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001A40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001A40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2389,7 +2389,7 @@
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001080000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3825,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C2" t="s">
         <v>356</v>
@@ -3836,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -7303,6 +7303,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C23:K23"/>
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="I24:J24"/>
@@ -7312,11 +7317,6 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7374,7 +7374,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7407,7 +7407,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -7415,7 +7415,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="45" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -7443,7 +7443,7 @@
       </c>
       <c r="B8" s="95" t="str">
         <f>CONCATENATE(B4,".",B5,"@mailinator.com")</f>
-        <v>Armando	.Bowers@mailinator.com</v>
+        <v>spijgsdj.skdjfspdjf@mailinator.com</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
@@ -7567,7 +7567,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -7575,7 +7575,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -8346,7 +8346,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -8354,7 +8354,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -9174,7 +9174,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -9182,7 +9182,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -10264,7 +10264,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C2" t="s">
         <v>356</v>
@@ -10275,7 +10275,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -10776,7 +10776,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -10784,7 +10784,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>
@@ -11547,7 +11547,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -11555,7 +11555,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="45" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>169</v>

</xml_diff>